<commit_message>
- TL (see git commit) - Fix how <nopause> is handled: TODO re-visit old scripts that use it to make sure they don't crash
</commit_message>
<xml_diff>
--- a/tl/S10048.MES.BIN.xlsx
+++ b/tl/S10048.MES.BIN.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6682AD-53C4-4449-9D49-89D272D2837C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1500B8F-EF7F-42CA-A758-849C1ED41E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="5460" windowWidth="55215" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3900" windowWidth="57615" windowHeight="13350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S10048.MES.BIN" sheetId="1" r:id="rId1"/>

</xml_diff>